<commit_message>
updated to hex grid from square grid using h3 library
</commit_message>
<xml_diff>
--- a/data/routes/jctsl_routes.xlsx
+++ b/data/routes/jctsl_routes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\P70087882\PycharmProjects\JCTSL-PTAL\data\routes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D407086C-319D-430D-9558-9F3828218FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1627483C-F769-417E-9012-466D16654E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{C8876AAD-A1CC-40D5-BFF5-CCC612A8B159}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="91">
   <si>
     <t>URBAN</t>
   </si>
@@ -304,6 +304,12 @@
   <si>
     <t>Tourist &amp; Airport Service</t>
   </si>
+  <si>
+    <t>25A</t>
+  </si>
+  <si>
+    <t>25B</t>
+  </si>
 </sst>
 </file>
 
@@ -345,7 +351,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -368,37 +374,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -422,36 +402,13 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -766,10 +723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFDAD641-AF38-4383-95F5-298B7DB5F470}">
-  <dimension ref="A1:AB997"/>
+  <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,7 +735,7 @@
     <col min="2" max="2" width="6" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" style="8" customWidth="1"/>
-    <col min="5" max="5" width="64.42578125" style="18" customWidth="1"/>
+    <col min="5" max="5" width="64.42578125" style="9" customWidth="1"/>
     <col min="6" max="6" width="8.42578125" style="8" customWidth="1"/>
     <col min="7" max="7" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5703125" style="8" customWidth="1"/>
@@ -962,7 +919,7 @@
       <c r="D4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="10" t="s">
         <v>52</v>
       </c>
       <c r="F4" s="4">
@@ -1012,7 +969,7 @@
       <c r="D5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="10" t="s">
         <v>53</v>
       </c>
       <c r="F5" s="4">
@@ -1062,7 +1019,7 @@
       <c r="D6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="10" t="s">
         <v>55</v>
       </c>
       <c r="F6" s="4">
@@ -1097,35 +1054,33 @@
       <c r="AA6" s="7"/>
       <c r="AB6" s="7"/>
     </row>
-    <row r="7" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>8</v>
+      <c r="B7" s="4">
+        <v>27</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" s="9">
+      <c r="E7" s="10"/>
+      <c r="F7" s="4">
         <v>48</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="4">
         <v>30</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="3">
         <v>4</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="I7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="12"/>
+      <c r="J7" s="5"/>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
@@ -1145,33 +1100,35 @@
       <c r="AA7" s="7"/>
       <c r="AB7" s="7"/>
     </row>
-    <row r="8" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="13">
-        <v>14</v>
+      <c r="D8" s="6" t="s">
+        <v>25</v>
       </c>
-      <c r="C8" s="14" t="s">
-        <v>7</v>
+      <c r="E8" s="10" t="s">
+        <v>54</v>
       </c>
-      <c r="D8" s="15" t="s">
-        <v>26</v>
+      <c r="F8" s="4">
+        <v>48</v>
       </c>
-      <c r="E8" s="17" t="s">
-        <v>56</v>
+      <c r="G8" s="4">
+        <v>30</v>
       </c>
-      <c r="F8" s="14">
-        <v>47</v>
+      <c r="H8" s="3">
+        <v>4</v>
       </c>
-      <c r="G8" s="14">
-        <v>15</v>
+      <c r="I8" s="5" t="s">
+        <v>6</v>
       </c>
-      <c r="H8" s="13"/>
-      <c r="I8" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="16"/>
+      <c r="J8" s="5"/>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
@@ -1193,29 +1150,27 @@
     </row>
     <row r="9" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
-      <c r="B9" s="4">
-        <v>26</v>
+      <c r="B9" s="3">
+        <v>14</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
-      <c r="E9" s="17" t="s">
-        <v>57</v>
+      <c r="E9" s="10" t="s">
+        <v>56</v>
       </c>
       <c r="F9" s="4">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="G9" s="4">
-        <v>20</v>
+        <v>15</v>
       </c>
-      <c r="H9" s="3">
-        <v>9</v>
-      </c>
+      <c r="H9" s="3"/>
       <c r="I9" s="5" t="s">
         <v>9</v>
       </c>
@@ -1241,35 +1196,33 @@
     </row>
     <row r="10" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="4">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
-      <c r="E10" s="17" t="s">
-        <v>58</v>
+      <c r="E10" s="10" t="s">
+        <v>57</v>
       </c>
       <c r="F10" s="4">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="G10" s="4">
         <v>20</v>
       </c>
       <c r="H10" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J10" s="5" t="s">
-        <v>85</v>
-      </c>
+      <c r="J10" s="5"/>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
@@ -1289,30 +1242,30 @@
       <c r="AA10" s="7"/>
       <c r="AB10" s="7"/>
     </row>
-    <row r="11" spans="1:28" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="4">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
-      <c r="E11" s="17" t="s">
-        <v>59</v>
+      <c r="E11" s="10" t="s">
+        <v>58</v>
       </c>
       <c r="F11" s="4">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G11" s="4">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="H11" s="3">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>9</v>
@@ -1339,36 +1292,36 @@
       <c r="AA11" s="7"/>
       <c r="AB11" s="7"/>
     </row>
-    <row r="12" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>11</v>
+        <v>10</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>1</v>
+      <c r="B12" s="4">
+        <v>7</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
-      <c r="E12" t="s">
-        <v>60</v>
+      <c r="E12" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="F12" s="4">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G12" s="4">
         <v>8</v>
       </c>
       <c r="H12" s="3">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>9</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
@@ -1391,33 +1344,35 @@
     </row>
     <row r="13" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
-      <c r="E13" t="s">
-        <v>61</v>
+      <c r="E13" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="F13" s="4">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G13" s="4">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="H13" s="3">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J13" s="5"/>
+      <c r="J13" s="5" t="s">
+        <v>87</v>
+      </c>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
@@ -1439,19 +1394,19 @@
     </row>
     <row r="14" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <v>13</v>
+        <v>12</v>
       </c>
-      <c r="B14" s="4">
-        <v>15</v>
+      <c r="B14" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
-      <c r="E14" t="s">
-        <v>62</v>
+      <c r="E14" s="11" t="s">
+        <v>61</v>
       </c>
       <c r="F14" s="4">
         <v>32</v>
@@ -1460,7 +1415,7 @@
         <v>20</v>
       </c>
       <c r="H14" s="3">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>9</v>
@@ -1487,28 +1442,28 @@
     </row>
     <row r="15" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="4">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
-      <c r="E15" t="s">
-        <v>63</v>
+      <c r="E15" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="F15" s="4">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G15" s="4">
         <v>20</v>
       </c>
       <c r="H15" s="3">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>9</v>
@@ -1535,28 +1490,28 @@
     </row>
     <row r="16" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="4">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
-      <c r="E16" t="s">
-        <v>64</v>
+      <c r="E16" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="F16" s="4">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G16" s="4">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="H16" s="3">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>9</v>
@@ -1583,28 +1538,28 @@
     </row>
     <row r="17" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="4">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>65</v>
+      <c r="E17" s="11" t="s">
+        <v>64</v>
       </c>
       <c r="F17" s="4">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="G17" s="4">
         <v>35</v>
       </c>
       <c r="H17" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>9</v>
@@ -1629,35 +1584,35 @@
       <c r="AA17" s="7"/>
       <c r="AB17" s="7"/>
     </row>
-    <row r="18" spans="1:28" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
-        <v>17</v>
+        <v>16</v>
       </c>
-      <c r="B18" s="9">
-        <v>34</v>
+      <c r="B18" s="4">
+        <v>24</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>0</v>
+      <c r="C18" s="4" t="s">
+        <v>2</v>
       </c>
-      <c r="D18" s="10" t="s">
-        <v>36</v>
+      <c r="D18" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="4">
+        <v>25</v>
+      </c>
+      <c r="G18" s="4">
         <v>35</v>
       </c>
-      <c r="G18" s="9">
-        <v>15</v>
+      <c r="H18" s="3">
+        <v>5</v>
       </c>
-      <c r="H18" s="11">
-        <v>14</v>
-      </c>
-      <c r="I18" s="12" t="s">
+      <c r="I18" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J18" s="12"/>
+      <c r="J18" s="5"/>
       <c r="K18" s="7"/>
       <c r="L18" s="7"/>
       <c r="M18" s="7"/>
@@ -1679,35 +1634,31 @@
     </row>
     <row r="19" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
-        <v>18</v>
+        <v>16</v>
       </c>
-      <c r="B19" s="14" t="s">
-        <v>10</v>
+      <c r="B19" s="4" t="s">
+        <v>89</v>
       </c>
-      <c r="C19" s="14" t="s">
-        <v>0</v>
+      <c r="C19" s="4" t="s">
+        <v>2</v>
       </c>
-      <c r="D19" s="15" t="s">
-        <v>37</v>
+      <c r="D19" s="6" t="s">
+        <v>35</v>
       </c>
-      <c r="E19" t="s">
-        <v>67</v>
+      <c r="E19" s="6"/>
+      <c r="F19" s="4">
+        <v>25</v>
       </c>
-      <c r="F19" s="14">
-        <v>21</v>
+      <c r="G19" s="4">
+        <v>35</v>
       </c>
-      <c r="G19" s="14">
-        <v>20</v>
-      </c>
-      <c r="H19" s="13">
-        <v>7</v>
-      </c>
-      <c r="I19" s="16" t="s">
+      <c r="H19" s="3">
         <v>5</v>
       </c>
-      <c r="J19" s="16" t="s">
-        <v>85</v>
+      <c r="I19" s="5" t="s">
+        <v>9</v>
       </c>
+      <c r="J19" s="5"/>
       <c r="K19" s="7"/>
       <c r="L19" s="7"/>
       <c r="M19" s="7"/>
@@ -1729,35 +1680,31 @@
     </row>
     <row r="20" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>3</v>
+        <v>90</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
-      <c r="E20" t="s">
-        <v>68</v>
-      </c>
+      <c r="E20" s="6"/>
       <c r="F20" s="4">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G20" s="4">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="H20" s="3">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
-      <c r="J20" s="5" t="s">
-        <v>85</v>
-      </c>
+      <c r="J20" s="5"/>
       <c r="K20" s="7"/>
       <c r="L20" s="7"/>
       <c r="M20" s="7"/>
@@ -1777,37 +1724,35 @@
       <c r="AA20" s="7"/>
       <c r="AB20" s="7"/>
     </row>
-    <row r="21" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
-        <v>20</v>
+        <v>17</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>11</v>
+      <c r="B21" s="4">
+        <v>34</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
-      <c r="E21" t="s">
-        <v>69</v>
+      <c r="E21" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="F21" s="4">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G21" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H21" s="3">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
-      <c r="J21" s="5" t="s">
-        <v>87</v>
-      </c>
+      <c r="J21" s="5"/>
       <c r="K21" s="7"/>
       <c r="L21" s="7"/>
       <c r="M21" s="7"/>
@@ -1829,25 +1774,25 @@
     </row>
     <row r="22" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>81</v>
+        <v>10</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
-      <c r="E22" t="s">
-        <v>70</v>
+      <c r="E22" s="11" t="s">
+        <v>67</v>
       </c>
       <c r="F22" s="4">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G22" s="4">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H22" s="3">
         <v>7</v>
@@ -1855,7 +1800,9 @@
       <c r="I22" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J22" s="5"/>
+      <c r="J22" s="5" t="s">
+        <v>85</v>
+      </c>
       <c r="K22" s="7"/>
       <c r="L22" s="7"/>
       <c r="M22" s="7"/>
@@ -1877,33 +1824,35 @@
     </row>
     <row r="23" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
-      <c r="E23" t="s">
-        <v>71</v>
+      <c r="E23" s="11" t="s">
+        <v>68</v>
       </c>
       <c r="F23" s="4">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G23" s="4">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H23" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J23" s="5"/>
+      <c r="J23" s="5" t="s">
+        <v>85</v>
+      </c>
       <c r="K23" s="7"/>
       <c r="L23" s="7"/>
       <c r="M23" s="7"/>
@@ -1925,33 +1874,35 @@
     </row>
     <row r="24" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
-        <v>23</v>
+        <v>20</v>
       </c>
-      <c r="B24" s="4">
-        <v>30</v>
+      <c r="B24" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
-      <c r="E24" s="6" t="s">
-        <v>72</v>
+      <c r="E24" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="F24" s="4">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G24" s="4">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="H24" s="3">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I24" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J24" s="5"/>
+      <c r="J24" s="5" t="s">
+        <v>87</v>
+      </c>
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
       <c r="M24" s="7"/>
@@ -1971,37 +1922,35 @@
       <c r="AA24" s="7"/>
       <c r="AB24" s="7"/>
     </row>
-    <row r="25" spans="1:28" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
-      <c r="E25" s="6" t="s">
-        <v>73</v>
+      <c r="E25" s="11" t="s">
+        <v>70</v>
       </c>
       <c r="F25" s="4">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="G25" s="4">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H25" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J25" s="5" t="s">
-        <v>88</v>
-      </c>
+      <c r="J25" s="5"/>
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
       <c r="M25" s="7"/>
@@ -2023,28 +1972,28 @@
     </row>
     <row r="26" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
-        <v>25</v>
+        <v>22</v>
       </c>
-      <c r="B26" s="3">
-        <v>11</v>
+      <c r="B26" s="4" t="s">
+        <v>82</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
-      <c r="E26" s="6" t="s">
-        <v>74</v>
+      <c r="E26" s="11" t="s">
+        <v>71</v>
       </c>
-      <c r="F26" s="3">
-        <v>27</v>
+      <c r="F26" s="4">
+        <v>17</v>
       </c>
-      <c r="G26" s="3">
-        <v>20</v>
+      <c r="G26" s="4">
+        <v>11</v>
       </c>
       <c r="H26" s="3">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="I26" s="5" t="s">
         <v>5</v>
@@ -2071,28 +2020,28 @@
     </row>
     <row r="27" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
-        <v>26</v>
+        <v>23</v>
       </c>
-      <c r="B27" s="3">
-        <v>18</v>
+      <c r="B27" s="4">
+        <v>30</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>0</v>
+      <c r="C27" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
-      <c r="F27" s="3">
-        <v>28</v>
+      <c r="F27" s="4">
+        <v>25</v>
       </c>
-      <c r="G27" s="3">
-        <v>50</v>
+      <c r="G27" s="4">
+        <v>20</v>
       </c>
       <c r="H27" s="3">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I27" s="5" t="s">
         <v>5</v>
@@ -2117,36 +2066,36 @@
       <c r="AA27" s="7"/>
       <c r="AB27" s="7"/>
     </row>
-    <row r="28" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
-        <v>27</v>
+        <v>24</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>4</v>
+      <c r="B28" s="4" t="s">
+        <v>83</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
-      <c r="E28" t="s">
-        <v>76</v>
+      <c r="E28" s="6" t="s">
+        <v>73</v>
       </c>
-      <c r="F28" s="3">
-        <v>26</v>
+      <c r="F28" s="4">
+        <v>28</v>
       </c>
-      <c r="G28" s="3">
-        <v>10</v>
+      <c r="G28" s="4">
+        <v>20</v>
       </c>
       <c r="H28" s="3">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="I28" s="5" t="s">
         <v>5</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
@@ -2169,35 +2118,33 @@
     </row>
     <row r="29" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
-        <v>28</v>
+        <v>25</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>12</v>
+      <c r="B29" s="3">
+        <v>11</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F29" s="3">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="G29" s="3">
         <v>20</v>
       </c>
       <c r="H29" s="3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I29" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J29" s="5" t="s">
-        <v>85</v>
-      </c>
+      <c r="J29" s="5"/>
       <c r="K29" s="7"/>
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
@@ -2217,17 +2164,35 @@
       <c r="AA29" s="7"/>
       <c r="AB29" s="7"/>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
+    <row r="30" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>26</v>
+      </c>
+      <c r="B30" s="3">
+        <v>18</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F30" s="3">
+        <v>28</v>
+      </c>
+      <c r="G30" s="3">
+        <v>50</v>
+      </c>
+      <c r="H30" s="3">
+        <v>2</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J30" s="5"/>
       <c r="K30" s="7"/>
       <c r="L30" s="7"/>
       <c r="M30" s="7"/>
@@ -2247,17 +2212,37 @@
       <c r="AA30" s="7"/>
       <c r="AB30" s="7"/>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
+    <row r="31" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>27</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F31" s="3">
+        <v>26</v>
+      </c>
+      <c r="G31" s="3">
+        <v>10</v>
+      </c>
+      <c r="H31" s="3">
+        <v>16</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>85</v>
+      </c>
       <c r="K31" s="7"/>
       <c r="L31" s="7"/>
       <c r="M31" s="7"/>
@@ -2277,17 +2262,37 @@
       <c r="AA31" s="7"/>
       <c r="AB31" s="7"/>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
+    <row r="32" spans="1:28" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>28</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F32" s="3">
+        <v>20</v>
+      </c>
+      <c r="G32" s="3">
+        <v>20</v>
+      </c>
+      <c r="H32" s="3">
+        <v>7</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>85</v>
+      </c>
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
@@ -2308,16 +2313,16 @@
       <c r="AB32" s="7"/>
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
+      <c r="A33" s="1"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
       <c r="M33" s="7"/>
@@ -31257,6 +31262,96 @@
       <c r="AA997" s="7"/>
       <c r="AB997" s="7"/>
     </row>
+    <row r="998" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A998" s="7"/>
+      <c r="B998" s="7"/>
+      <c r="C998" s="7"/>
+      <c r="D998" s="7"/>
+      <c r="E998" s="7"/>
+      <c r="F998" s="7"/>
+      <c r="G998" s="7"/>
+      <c r="H998" s="7"/>
+      <c r="I998" s="7"/>
+      <c r="J998" s="7"/>
+      <c r="K998" s="7"/>
+      <c r="L998" s="7"/>
+      <c r="M998" s="7"/>
+      <c r="N998" s="7"/>
+      <c r="O998" s="7"/>
+      <c r="P998" s="7"/>
+      <c r="Q998" s="7"/>
+      <c r="R998" s="7"/>
+      <c r="S998" s="7"/>
+      <c r="T998" s="7"/>
+      <c r="U998" s="7"/>
+      <c r="V998" s="7"/>
+      <c r="W998" s="7"/>
+      <c r="X998" s="7"/>
+      <c r="Y998" s="7"/>
+      <c r="Z998" s="7"/>
+      <c r="AA998" s="7"/>
+      <c r="AB998" s="7"/>
+    </row>
+    <row r="999" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A999" s="7"/>
+      <c r="B999" s="7"/>
+      <c r="C999" s="7"/>
+      <c r="D999" s="7"/>
+      <c r="E999" s="7"/>
+      <c r="F999" s="7"/>
+      <c r="G999" s="7"/>
+      <c r="H999" s="7"/>
+      <c r="I999" s="7"/>
+      <c r="J999" s="7"/>
+      <c r="K999" s="7"/>
+      <c r="L999" s="7"/>
+      <c r="M999" s="7"/>
+      <c r="N999" s="7"/>
+      <c r="O999" s="7"/>
+      <c r="P999" s="7"/>
+      <c r="Q999" s="7"/>
+      <c r="R999" s="7"/>
+      <c r="S999" s="7"/>
+      <c r="T999" s="7"/>
+      <c r="U999" s="7"/>
+      <c r="V999" s="7"/>
+      <c r="W999" s="7"/>
+      <c r="X999" s="7"/>
+      <c r="Y999" s="7"/>
+      <c r="Z999" s="7"/>
+      <c r="AA999" s="7"/>
+      <c r="AB999" s="7"/>
+    </row>
+    <row r="1000" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1000" s="7"/>
+      <c r="B1000" s="7"/>
+      <c r="C1000" s="7"/>
+      <c r="D1000" s="7"/>
+      <c r="E1000" s="7"/>
+      <c r="F1000" s="7"/>
+      <c r="G1000" s="7"/>
+      <c r="H1000" s="7"/>
+      <c r="I1000" s="7"/>
+      <c r="J1000" s="7"/>
+      <c r="K1000" s="7"/>
+      <c r="L1000" s="7"/>
+      <c r="M1000" s="7"/>
+      <c r="N1000" s="7"/>
+      <c r="O1000" s="7"/>
+      <c r="P1000" s="7"/>
+      <c r="Q1000" s="7"/>
+      <c r="R1000" s="7"/>
+      <c r="S1000" s="7"/>
+      <c r="T1000" s="7"/>
+      <c r="U1000" s="7"/>
+      <c r="V1000" s="7"/>
+      <c r="W1000" s="7"/>
+      <c r="X1000" s="7"/>
+      <c r="Y1000" s="7"/>
+      <c r="Z1000" s="7"/>
+      <c r="AA1000" s="7"/>
+      <c r="AB1000" s="7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>